<commit_message>
SON24 new content: Charts and tables: Composite Index: Promising Prospects: Review mark-ups
</commit_message>
<xml_diff>
--- a/son/content/intermediate_outcomes/composite_indices/promising_prospects/2.0/CI1-2.0-promising-prospects--by-region--chart-format.xlsx
+++ b/son/content/intermediate_outcomes/composite_indices/promising_prospects/2.0/CI1-2.0-promising-prospects--by-region--chart-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\intermediate_outcomes\composite_indices\promising_prospects\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05717C-D164-41F3-8093-1CDD57AC47C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C7F35-B6BF-44F0-B632-7666818B6124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{FF064F49-A2CC-412D-8776-399ED2BDA7A0}"/>
   </bookViews>
@@ -1713,7 +1713,7 @@
         <v>28</v>
       </c>
       <c r="M2">
-        <v>-7.1983713000000005E-2</v>
+        <v>7.1983713000000005E-2</v>
       </c>
       <c r="N2" t="s">
         <v>25</v>
@@ -1779,7 +1779,7 @@
         <v>28</v>
       </c>
       <c r="M3">
-        <v>-8.9618375E-2</v>
+        <v>8.9618375E-2</v>
       </c>
       <c r="N3" t="s">
         <v>25</v>
@@ -1851,7 +1851,7 @@
         <v>28</v>
       </c>
       <c r="M4">
-        <v>0.59514336499999998</v>
+        <v>-0.59514336499999998</v>
       </c>
       <c r="N4" t="s">
         <v>25</v>
@@ -1923,7 +1923,7 @@
         <v>28</v>
       </c>
       <c r="M5">
-        <v>0.32333544800000003</v>
+        <v>-0.32333544800000003</v>
       </c>
       <c r="N5" t="s">
         <v>25</v>
@@ -1995,7 +1995,7 @@
         <v>28</v>
       </c>
       <c r="M6">
-        <v>-0.261754388</v>
+        <v>0.261754388</v>
       </c>
       <c r="N6" t="s">
         <v>25</v>
@@ -2067,7 +2067,7 @@
         <v>28</v>
       </c>
       <c r="M7">
-        <v>-2.7366124350000001</v>
+        <v>2.7366124350000001</v>
       </c>
       <c r="N7" t="s">
         <v>25</v>
@@ -2139,7 +2139,7 @@
         <v>28</v>
       </c>
       <c r="M8">
-        <v>1.78919077</v>
+        <v>-1.78919077</v>
       </c>
       <c r="N8" t="s">
         <v>25</v>
@@ -2205,7 +2205,7 @@
         <v>28</v>
       </c>
       <c r="M9">
-        <v>-0.24769707399999999</v>
+        <v>0.24769707399999999</v>
       </c>
       <c r="N9" t="s">
         <v>25</v>
@@ -2271,7 +2271,7 @@
         <v>28</v>
       </c>
       <c r="M10">
-        <v>-1.7980608810000001</v>
+        <v>1.7980608810000001</v>
       </c>
       <c r="N10" t="s">
         <v>25</v>
@@ -2337,7 +2337,7 @@
         <v>28</v>
       </c>
       <c r="M11">
-        <v>-1.297692157</v>
+        <v>1.297692157</v>
       </c>
       <c r="N11" t="s">
         <v>25</v>
@@ -2403,7 +2403,7 @@
         <v>28</v>
       </c>
       <c r="M12">
-        <v>0.37539388600000001</v>
+        <v>-0.37539388600000001</v>
       </c>
       <c r="N12" t="s">
         <v>25</v>
@@ -2469,7 +2469,7 @@
         <v>28</v>
       </c>
       <c r="M13">
-        <v>0.47693346399999997</v>
+        <v>-0.47693346399999997</v>
       </c>
       <c r="N13" t="s">
         <v>25</v>
@@ -2535,7 +2535,7 @@
         <v>28</v>
       </c>
       <c r="M14">
-        <v>0.117437781</v>
+        <v>-0.117437781</v>
       </c>
       <c r="N14" t="s">
         <v>25</v>
@@ -2601,7 +2601,7 @@
         <v>28</v>
       </c>
       <c r="M15">
-        <v>0.58457993600000002</v>
+        <v>-0.58457993600000002</v>
       </c>
       <c r="N15" t="s">
         <v>25</v>
@@ -2667,7 +2667,7 @@
         <v>28</v>
       </c>
       <c r="M16">
-        <v>0.21556398399999999</v>
+        <v>-0.21556398399999999</v>
       </c>
       <c r="N16" t="s">
         <v>25</v>
@@ -2733,7 +2733,7 @@
         <v>28</v>
       </c>
       <c r="M17">
-        <v>-0.37671931800000003</v>
+        <v>0.37671931800000003</v>
       </c>
       <c r="N17" t="s">
         <v>25</v>
@@ -2799,7 +2799,7 @@
         <v>28</v>
       </c>
       <c r="M18">
-        <v>-0.74603320900000003</v>
+        <v>0.74603320900000003</v>
       </c>
       <c r="N18" t="s">
         <v>25</v>
@@ -2865,7 +2865,7 @@
         <v>28</v>
       </c>
       <c r="M19">
-        <v>0.863818274</v>
+        <v>-0.863818274</v>
       </c>
       <c r="N19" t="s">
         <v>25</v>
@@ -2931,7 +2931,7 @@
         <v>28</v>
       </c>
       <c r="M20">
-        <v>-2.5957575030000002</v>
+        <v>2.5957575030000002</v>
       </c>
       <c r="N20" t="s">
         <v>25</v>
@@ -2997,7 +2997,7 @@
         <v>28</v>
       </c>
       <c r="M21">
-        <v>0.76526300300000005</v>
+        <v>-0.76526300300000005</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>
@@ -3063,7 +3063,7 @@
         <v>28</v>
       </c>
       <c r="M22">
-        <v>-1.2230650059999999</v>
+        <v>1.2230650059999999</v>
       </c>
       <c r="N22" t="s">
         <v>25</v>
@@ -3129,7 +3129,7 @@
         <v>28</v>
       </c>
       <c r="M23">
-        <v>0.13227166000000001</v>
+        <v>-0.13227166000000001</v>
       </c>
       <c r="N23" t="s">
         <v>25</v>
@@ -3195,7 +3195,7 @@
         <v>28</v>
       </c>
       <c r="M24">
-        <v>-0.950306647</v>
+        <v>0.950306647</v>
       </c>
       <c r="N24" t="s">
         <v>25</v>
@@ -3261,7 +3261,7 @@
         <v>28</v>
       </c>
       <c r="M25">
-        <v>-1.828132737</v>
+        <v>1.828132737</v>
       </c>
       <c r="N25" t="s">
         <v>25</v>
@@ -3327,7 +3327,7 @@
         <v>28</v>
       </c>
       <c r="M26">
-        <v>0.41822131400000001</v>
+        <v>-0.41822131400000001</v>
       </c>
       <c r="N26" t="s">
         <v>25</v>
@@ -3393,7 +3393,7 @@
         <v>28</v>
       </c>
       <c r="M27">
-        <v>0.91985742299999995</v>
+        <v>-0.91985742299999995</v>
       </c>
       <c r="N27" t="s">
         <v>25</v>
@@ -3459,7 +3459,7 @@
         <v>28</v>
       </c>
       <c r="M28">
-        <v>0.21759357900000001</v>
+        <v>-0.21759357900000001</v>
       </c>
       <c r="N28" t="s">
         <v>25</v>
@@ -3525,7 +3525,7 @@
         <v>28</v>
       </c>
       <c r="M29">
-        <v>0.46221678399999999</v>
+        <v>-0.46221678399999999</v>
       </c>
       <c r="N29" t="s">
         <v>25</v>
@@ -3591,7 +3591,7 @@
         <v>28</v>
       </c>
       <c r="M30">
-        <v>-2.0689722580000001</v>
+        <v>2.0689722580000001</v>
       </c>
       <c r="N30" t="s">
         <v>25</v>
@@ -3657,7 +3657,7 @@
         <v>28</v>
       </c>
       <c r="M31">
-        <v>0.445109374</v>
+        <v>-0.445109374</v>
       </c>
       <c r="N31" t="s">
         <v>25</v>
@@ -3723,7 +3723,7 @@
         <v>28</v>
       </c>
       <c r="M32">
-        <v>0.32049246300000001</v>
+        <v>-0.32049246300000001</v>
       </c>
       <c r="N32" t="s">
         <v>25</v>
@@ -3789,7 +3789,7 @@
         <v>28</v>
       </c>
       <c r="M33">
-        <v>-1.4209266730000001</v>
+        <v>1.4209266730000001</v>
       </c>
       <c r="N33" t="s">
         <v>25</v>
@@ -3855,7 +3855,7 @@
         <v>28</v>
       </c>
       <c r="M34">
-        <v>0.51644716000000002</v>
+        <v>-0.51644716000000002</v>
       </c>
       <c r="N34" t="s">
         <v>25</v>
@@ -3921,7 +3921,7 @@
         <v>28</v>
       </c>
       <c r="M35">
-        <v>-1.0086590369999999</v>
+        <v>1.0086590369999999</v>
       </c>
       <c r="N35" t="s">
         <v>25</v>
@@ -3987,7 +3987,7 @@
         <v>28</v>
       </c>
       <c r="M36">
-        <v>0.59312735999999999</v>
+        <v>-0.59312735999999999</v>
       </c>
       <c r="N36" t="s">
         <v>25</v>
@@ -4053,7 +4053,7 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>-0.81674992000000002</v>
+        <v>0.81674992000000002</v>
       </c>
       <c r="N37" t="s">
         <v>25</v>
@@ -4119,7 +4119,7 @@
         <v>28</v>
       </c>
       <c r="M38">
-        <v>0.72718787600000001</v>
+        <v>-0.72718787600000001</v>
       </c>
       <c r="N38" t="s">
         <v>25</v>
@@ -4185,7 +4185,7 @@
         <v>28</v>
       </c>
       <c r="M39">
-        <v>0.26034648700000002</v>
+        <v>-0.26034648700000002</v>
       </c>
       <c r="N39" t="s">
         <v>25</v>
@@ -4251,7 +4251,7 @@
         <v>28</v>
       </c>
       <c r="M40">
-        <v>1.4017197219999999</v>
+        <v>-1.4017197219999999</v>
       </c>
       <c r="N40" t="s">
         <v>25</v>
@@ -4317,7 +4317,7 @@
         <v>28</v>
       </c>
       <c r="M41">
-        <v>0.87017839500000005</v>
+        <v>-0.87017839500000005</v>
       </c>
       <c r="N41" t="s">
         <v>25</v>
@@ -4383,7 +4383,7 @@
         <v>28</v>
       </c>
       <c r="M42">
-        <v>-0.96599149299999998</v>
+        <v>0.96599149299999998</v>
       </c>
       <c r="N42" t="s">
         <v>25</v>
@@ -4449,7 +4449,7 @@
         <v>28</v>
       </c>
       <c r="M43">
-        <v>0.79403447599999999</v>
+        <v>-0.79403447599999999</v>
       </c>
       <c r="N43" t="s">
         <v>25</v>
@@ -4515,7 +4515,7 @@
         <v>28</v>
       </c>
       <c r="M44">
-        <v>0.40671806799999999</v>
+        <v>-0.40671806799999999</v>
       </c>
       <c r="N44" t="s">
         <v>25</v>
@@ -4581,7 +4581,7 @@
         <v>28</v>
       </c>
       <c r="M45">
-        <v>0.45864543600000002</v>
+        <v>-0.45864543600000002</v>
       </c>
       <c r="N45" t="s">
         <v>25</v>
@@ -4647,7 +4647,7 @@
         <v>28</v>
       </c>
       <c r="M46">
-        <v>0.21205392100000001</v>
+        <v>-0.21205392100000001</v>
       </c>
       <c r="N46" t="s">
         <v>25</v>
@@ -4713,7 +4713,7 @@
         <v>28</v>
       </c>
       <c r="M47">
-        <v>0.237658698</v>
+        <v>-0.237658698</v>
       </c>
       <c r="N47" t="s">
         <v>25</v>
@@ -4779,7 +4779,7 @@
         <v>28</v>
       </c>
       <c r="M48">
-        <v>-0.13959798900000001</v>
+        <v>0.13959798900000001</v>
       </c>
       <c r="N48" t="s">
         <v>25</v>
@@ -4845,7 +4845,7 @@
         <v>28</v>
       </c>
       <c r="M49">
-        <v>0.90066563700000002</v>
+        <v>-0.90066563700000002</v>
       </c>
       <c r="N49" t="s">
         <v>25</v>
@@ -4911,7 +4911,7 @@
         <v>28</v>
       </c>
       <c r="M50">
-        <v>-1.490299E-2</v>
+        <v>1.490299E-2</v>
       </c>
       <c r="N50" t="s">
         <v>25</v>
@@ -4977,7 +4977,7 @@
         <v>28</v>
       </c>
       <c r="M51">
-        <v>0.233613931</v>
+        <v>-0.233613931</v>
       </c>
       <c r="N51" t="s">
         <v>25</v>
@@ -5043,7 +5043,7 @@
         <v>28</v>
       </c>
       <c r="M52">
-        <v>1.5504309810000001</v>
+        <v>-1.5504309810000001</v>
       </c>
       <c r="N52" t="s">
         <v>25</v>
@@ -5109,7 +5109,7 @@
         <v>28</v>
       </c>
       <c r="M53">
-        <v>0.33939468099999998</v>
+        <v>-0.33939468099999998</v>
       </c>
       <c r="N53" t="s">
         <v>25</v>
@@ -5175,7 +5175,7 @@
         <v>28</v>
       </c>
       <c r="M54">
-        <v>1.6985861330000001</v>
+        <v>-1.6985861330000001</v>
       </c>
       <c r="N54" t="s">
         <v>25</v>
@@ -5241,7 +5241,7 @@
         <v>28</v>
       </c>
       <c r="M55">
-        <v>-2.8594093109999998</v>
+        <v>2.8594093109999998</v>
       </c>
       <c r="N55" t="s">
         <v>25</v>
@@ -5307,7 +5307,7 @@
         <v>28</v>
       </c>
       <c r="M56">
-        <v>1.0310463809999999</v>
+        <v>-1.0310463809999999</v>
       </c>
       <c r="N56" t="s">
         <v>25</v>
@@ -5373,7 +5373,7 @@
         <v>28</v>
       </c>
       <c r="M57">
-        <v>0.85702756899999999</v>
+        <v>-0.85702756899999999</v>
       </c>
       <c r="N57" t="s">
         <v>25</v>
@@ -5439,7 +5439,7 @@
         <v>28</v>
       </c>
       <c r="M58">
-        <v>0.276933135</v>
+        <v>-0.276933135</v>
       </c>
       <c r="N58" t="s">
         <v>25</v>
@@ -5505,7 +5505,7 @@
         <v>28</v>
       </c>
       <c r="M59">
-        <v>0.63265239600000001</v>
+        <v>-0.63265239600000001</v>
       </c>
       <c r="N59" t="s">
         <v>25</v>
@@ -5571,7 +5571,7 @@
         <v>28</v>
       </c>
       <c r="M60">
-        <v>0.52084005300000003</v>
+        <v>-0.52084005300000003</v>
       </c>
       <c r="N60" t="s">
         <v>25</v>
@@ -5637,7 +5637,7 @@
         <v>28</v>
       </c>
       <c r="M61">
-        <v>-0.61115986</v>
+        <v>0.61115986</v>
       </c>
       <c r="N61" t="s">
         <v>25</v>
@@ -5703,7 +5703,7 @@
         <v>28</v>
       </c>
       <c r="M62">
-        <v>-1.3879397659999999</v>
+        <v>1.3879397659999999</v>
       </c>
       <c r="N62" t="s">
         <v>25</v>
@@ -5769,7 +5769,7 @@
         <v>28</v>
       </c>
       <c r="M63">
-        <v>-0.36419370099999998</v>
+        <v>0.36419370099999998</v>
       </c>
       <c r="N63" t="s">
         <v>25</v>
@@ -5835,7 +5835,7 @@
         <v>28</v>
       </c>
       <c r="M64">
-        <v>0.76002512799999999</v>
+        <v>-0.76002512799999999</v>
       </c>
       <c r="N64" t="s">
         <v>25</v>
@@ -5901,7 +5901,7 @@
         <v>28</v>
       </c>
       <c r="M65">
-        <v>0.98858030699999999</v>
+        <v>-0.98858030699999999</v>
       </c>
       <c r="N65" t="s">
         <v>25</v>
@@ -5967,7 +5967,7 @@
         <v>28</v>
       </c>
       <c r="M66">
-        <v>0.406783381</v>
+        <v>-0.406783381</v>
       </c>
       <c r="N66" t="s">
         <v>25</v>
@@ -6033,7 +6033,7 @@
         <v>28</v>
       </c>
       <c r="M67">
-        <v>1.5780220890000001</v>
+        <v>-1.5780220890000001</v>
       </c>
       <c r="N67" t="s">
         <v>25</v>
@@ -6099,7 +6099,7 @@
         <v>28</v>
       </c>
       <c r="M68">
-        <v>0.840401917</v>
+        <v>-0.840401917</v>
       </c>
       <c r="N68" t="s">
         <v>25</v>
@@ -6165,7 +6165,7 @@
         <v>28</v>
       </c>
       <c r="M69">
-        <v>-0.53651669499999999</v>
+        <v>0.53651669499999999</v>
       </c>
       <c r="N69" t="s">
         <v>25</v>
@@ -6231,7 +6231,7 @@
         <v>28</v>
       </c>
       <c r="M70">
-        <v>-0.96530922600000002</v>
+        <v>0.96530922600000002</v>
       </c>
       <c r="N70" t="s">
         <v>25</v>
@@ -6297,7 +6297,7 @@
         <v>28</v>
       </c>
       <c r="M71">
-        <v>0.43304602599999997</v>
+        <v>-0.43304602599999997</v>
       </c>
       <c r="N71" t="s">
         <v>25</v>
@@ -6363,7 +6363,7 @@
         <v>28</v>
       </c>
       <c r="M72">
-        <v>-1.455764984</v>
+        <v>1.455764984</v>
       </c>
       <c r="N72" t="s">
         <v>25</v>
@@ -6429,7 +6429,7 @@
         <v>28</v>
       </c>
       <c r="M73">
-        <v>0.537048788</v>
+        <v>-0.537048788</v>
       </c>
       <c r="N73" t="s">
         <v>25</v>
@@ -6495,7 +6495,7 @@
         <v>28</v>
       </c>
       <c r="M74">
-        <v>-1.33685429</v>
+        <v>1.33685429</v>
       </c>
       <c r="N74" t="s">
         <v>25</v>
@@ -6561,7 +6561,7 @@
         <v>28</v>
       </c>
       <c r="M75">
-        <v>-0.59549723700000001</v>
+        <v>0.59549723700000001</v>
       </c>
       <c r="N75" t="s">
         <v>25</v>
@@ -6627,7 +6627,7 @@
         <v>28</v>
       </c>
       <c r="M76">
-        <v>-1.39315703</v>
+        <v>1.39315703</v>
       </c>
       <c r="N76" t="s">
         <v>25</v>
@@ -6693,7 +6693,7 @@
         <v>28</v>
       </c>
       <c r="M77">
-        <v>-2.8827869160000001</v>
+        <v>2.8827869160000001</v>
       </c>
       <c r="N77" t="s">
         <v>25</v>
@@ -6759,7 +6759,7 @@
         <v>28</v>
       </c>
       <c r="M78">
-        <v>1.079522745</v>
+        <v>-1.079522745</v>
       </c>
       <c r="N78" t="s">
         <v>25</v>
@@ -6825,7 +6825,7 @@
         <v>28</v>
       </c>
       <c r="M79">
-        <v>-0.67827490599999996</v>
+        <v>0.67827490599999996</v>
       </c>
       <c r="N79" t="s">
         <v>25</v>
@@ -6891,7 +6891,7 @@
         <v>28</v>
       </c>
       <c r="M80">
-        <v>-0.94993249000000002</v>
+        <v>0.94993249000000002</v>
       </c>
       <c r="N80" t="s">
         <v>25</v>
@@ -6957,7 +6957,7 @@
         <v>28</v>
       </c>
       <c r="M81">
-        <v>-1.8320347480000001</v>
+        <v>1.8320347480000001</v>
       </c>
       <c r="N81" t="s">
         <v>25</v>
@@ -7023,7 +7023,7 @@
         <v>28</v>
       </c>
       <c r="M82">
-        <v>0.26200470399999998</v>
+        <v>-0.26200470399999998</v>
       </c>
       <c r="N82" t="s">
         <v>25</v>
@@ -7089,7 +7089,7 @@
         <v>28</v>
       </c>
       <c r="M83">
-        <v>-2.166028544</v>
+        <v>2.166028544</v>
       </c>
       <c r="N83" t="s">
         <v>25</v>
@@ -7155,7 +7155,7 @@
         <v>28</v>
       </c>
       <c r="M84">
-        <v>-2.8450292309999998</v>
+        <v>2.8450292309999998</v>
       </c>
       <c r="N84" t="s">
         <v>25</v>
@@ -7221,7 +7221,7 @@
         <v>28</v>
       </c>
       <c r="M85">
-        <v>0.95193659600000002</v>
+        <v>-0.95193659600000002</v>
       </c>
       <c r="N85" t="s">
         <v>25</v>
@@ -7287,7 +7287,7 @@
         <v>28</v>
       </c>
       <c r="M86">
-        <v>0.45714067400000002</v>
+        <v>-0.45714067400000002</v>
       </c>
       <c r="N86" t="s">
         <v>25</v>
@@ -7353,7 +7353,7 @@
         <v>28</v>
       </c>
       <c r="M87">
-        <v>-0.15847351600000001</v>
+        <v>0.15847351600000001</v>
       </c>
       <c r="N87" t="s">
         <v>25</v>
@@ -7419,7 +7419,7 @@
         <v>28</v>
       </c>
       <c r="M88">
-        <v>-1.373330551</v>
+        <v>1.373330551</v>
       </c>
       <c r="N88" t="s">
         <v>25</v>
@@ -7485,7 +7485,7 @@
         <v>28</v>
       </c>
       <c r="M89">
-        <v>-1.4863867319999999</v>
+        <v>1.4863867319999999</v>
       </c>
       <c r="N89" t="s">
         <v>25</v>
@@ -7551,7 +7551,7 @@
         <v>28</v>
       </c>
       <c r="M90">
-        <v>-0.59521580100000004</v>
+        <v>0.59521580100000004</v>
       </c>
       <c r="N90" t="s">
         <v>25</v>
@@ -7617,7 +7617,7 @@
         <v>28</v>
       </c>
       <c r="M91">
-        <v>1.1993247520000001</v>
+        <v>-1.1993247520000001</v>
       </c>
       <c r="N91" t="s">
         <v>25</v>
@@ -7683,7 +7683,7 @@
         <v>28</v>
       </c>
       <c r="M92">
-        <v>-1.059997294</v>
+        <v>1.059997294</v>
       </c>
       <c r="N92" t="s">
         <v>25</v>
@@ -7749,7 +7749,7 @@
         <v>28</v>
       </c>
       <c r="M93">
-        <v>1.0206778329999999</v>
+        <v>-1.0206778329999999</v>
       </c>
       <c r="N93" t="s">
         <v>25</v>
@@ -7815,7 +7815,7 @@
         <v>28</v>
       </c>
       <c r="M94">
-        <v>0.59688655199999996</v>
+        <v>-0.59688655199999996</v>
       </c>
       <c r="N94" t="s">
         <v>25</v>
@@ -7881,7 +7881,7 @@
         <v>28</v>
       </c>
       <c r="M95">
-        <v>-1.5948321670000001</v>
+        <v>1.5948321670000001</v>
       </c>
       <c r="N95" t="s">
         <v>25</v>
@@ -7947,7 +7947,7 @@
         <v>28</v>
       </c>
       <c r="M96">
-        <v>0.42400996099999999</v>
+        <v>-0.42400996099999999</v>
       </c>
       <c r="N96" t="s">
         <v>25</v>
@@ -8013,7 +8013,7 @@
         <v>28</v>
       </c>
       <c r="M97">
-        <v>0.20578817199999999</v>
+        <v>-0.20578817199999999</v>
       </c>
       <c r="N97" t="s">
         <v>25</v>
@@ -8079,7 +8079,7 @@
         <v>28</v>
       </c>
       <c r="M98">
-        <v>-0.59909649600000003</v>
+        <v>0.59909649600000003</v>
       </c>
       <c r="N98" t="s">
         <v>25</v>
@@ -8145,7 +8145,7 @@
         <v>28</v>
       </c>
       <c r="M99">
-        <v>-0.10471688799999999</v>
+        <v>0.10471688799999999</v>
       </c>
       <c r="N99" t="s">
         <v>25</v>
@@ -8211,7 +8211,7 @@
         <v>28</v>
       </c>
       <c r="M100">
-        <v>-1.363451776</v>
+        <v>1.363451776</v>
       </c>
       <c r="N100" t="s">
         <v>25</v>
@@ -8277,7 +8277,7 @@
         <v>28</v>
       </c>
       <c r="M101">
-        <v>0.67879238900000005</v>
+        <v>-0.67879238900000005</v>
       </c>
       <c r="N101" t="s">
         <v>25</v>
@@ -8343,7 +8343,7 @@
         <v>28</v>
       </c>
       <c r="M102">
-        <v>0.28867956900000002</v>
+        <v>-0.28867956900000002</v>
       </c>
       <c r="N102" t="s">
         <v>25</v>
@@ -8409,7 +8409,7 @@
         <v>28</v>
       </c>
       <c r="M103">
-        <v>-1.33592399</v>
+        <v>1.33592399</v>
       </c>
       <c r="N103" t="s">
         <v>25</v>
@@ -8475,7 +8475,7 @@
         <v>28</v>
       </c>
       <c r="M104">
-        <v>0.21641250500000001</v>
+        <v>-0.21641250500000001</v>
       </c>
       <c r="N104" t="s">
         <v>25</v>
@@ -8541,7 +8541,7 @@
         <v>28</v>
       </c>
       <c r="M105">
-        <v>0.30270980400000003</v>
+        <v>-0.30270980400000003</v>
       </c>
       <c r="N105" t="s">
         <v>25</v>
@@ -8607,7 +8607,7 @@
         <v>28</v>
       </c>
       <c r="M106">
-        <v>0.37353966300000002</v>
+        <v>-0.37353966300000002</v>
       </c>
       <c r="N106" t="s">
         <v>25</v>
@@ -8673,7 +8673,7 @@
         <v>28</v>
       </c>
       <c r="M107">
-        <v>-0.83087828699999999</v>
+        <v>0.83087828699999999</v>
       </c>
       <c r="N107" t="s">
         <v>25</v>
@@ -8739,7 +8739,7 @@
         <v>28</v>
       </c>
       <c r="M108">
-        <v>0.44509143200000001</v>
+        <v>-0.44509143200000001</v>
       </c>
       <c r="N108" t="s">
         <v>25</v>
@@ -8805,7 +8805,7 @@
         <v>28</v>
       </c>
       <c r="M109">
-        <v>0.52447365499999998</v>
+        <v>-0.52447365499999998</v>
       </c>
       <c r="N109" t="s">
         <v>25</v>
@@ -8871,7 +8871,7 @@
         <v>28</v>
       </c>
       <c r="M110">
-        <v>-0.97626729400000001</v>
+        <v>0.97626729400000001</v>
       </c>
       <c r="N110" t="s">
         <v>25</v>
@@ -8937,7 +8937,7 @@
         <v>28</v>
       </c>
       <c r="M111">
-        <v>0.492901225</v>
+        <v>-0.492901225</v>
       </c>
       <c r="N111" t="s">
         <v>25</v>
@@ -9003,7 +9003,7 @@
         <v>28</v>
       </c>
       <c r="M112">
-        <v>0.40880140300000001</v>
+        <v>-0.40880140300000001</v>
       </c>
       <c r="N112" t="s">
         <v>25</v>
@@ -9069,7 +9069,7 @@
         <v>28</v>
       </c>
       <c r="M113">
-        <v>0.43793707799999998</v>
+        <v>-0.43793707799999998</v>
       </c>
       <c r="N113" t="s">
         <v>25</v>
@@ -9135,7 +9135,7 @@
         <v>28</v>
       </c>
       <c r="M114">
-        <v>0.50367129200000005</v>
+        <v>-0.50367129200000005</v>
       </c>
       <c r="N114" t="s">
         <v>25</v>
@@ -9201,7 +9201,7 @@
         <v>28</v>
       </c>
       <c r="M115">
-        <v>1.1570522999999999</v>
+        <v>-1.1570522999999999</v>
       </c>
       <c r="N115" t="s">
         <v>25</v>
@@ -9267,7 +9267,7 @@
         <v>28</v>
       </c>
       <c r="M116">
-        <v>-1.263887429</v>
+        <v>1.263887429</v>
       </c>
       <c r="N116" t="s">
         <v>25</v>
@@ -9333,7 +9333,7 @@
         <v>28</v>
       </c>
       <c r="M117">
-        <v>0.50175100500000003</v>
+        <v>-0.50175100500000003</v>
       </c>
       <c r="N117" t="s">
         <v>25</v>
@@ -9399,7 +9399,7 @@
         <v>28</v>
       </c>
       <c r="M118">
-        <v>1.094311021</v>
+        <v>-1.094311021</v>
       </c>
       <c r="N118" t="s">
         <v>25</v>
@@ -9465,7 +9465,7 @@
         <v>28</v>
       </c>
       <c r="M119">
-        <v>1.1094110450000001</v>
+        <v>-1.1094110450000001</v>
       </c>
       <c r="N119" t="s">
         <v>25</v>
@@ -9531,7 +9531,7 @@
         <v>28</v>
       </c>
       <c r="M120">
-        <v>1.964888865</v>
+        <v>-1.964888865</v>
       </c>
       <c r="N120" t="s">
         <v>25</v>
@@ -9597,7 +9597,7 @@
         <v>28</v>
       </c>
       <c r="M121">
-        <v>0.88599317600000005</v>
+        <v>-0.88599317600000005</v>
       </c>
       <c r="N121" t="s">
         <v>25</v>
@@ -9663,7 +9663,7 @@
         <v>28</v>
       </c>
       <c r="M122">
-        <v>0.86578149100000001</v>
+        <v>-0.86578149100000001</v>
       </c>
       <c r="N122" t="s">
         <v>25</v>
@@ -9729,7 +9729,7 @@
         <v>28</v>
       </c>
       <c r="M123">
-        <v>1.1495821909999999</v>
+        <v>-1.1495821909999999</v>
       </c>
       <c r="N123" t="s">
         <v>25</v>
@@ -9795,7 +9795,7 @@
         <v>28</v>
       </c>
       <c r="M124">
-        <v>0.13066381899999999</v>
+        <v>-0.13066381899999999</v>
       </c>
       <c r="N124" t="s">
         <v>25</v>
@@ -9861,7 +9861,7 @@
         <v>28</v>
       </c>
       <c r="M125">
-        <v>1.5246730669999999</v>
+        <v>-1.5246730669999999</v>
       </c>
       <c r="N125" t="s">
         <v>25</v>
@@ -9927,7 +9927,7 @@
         <v>28</v>
       </c>
       <c r="M126">
-        <v>1.381388356</v>
+        <v>-1.381388356</v>
       </c>
       <c r="N126" t="s">
         <v>25</v>
@@ -9993,7 +9993,7 @@
         <v>28</v>
       </c>
       <c r="M127">
-        <v>0.31564293900000001</v>
+        <v>-0.31564293900000001</v>
       </c>
       <c r="N127" t="s">
         <v>25</v>
@@ -10059,7 +10059,7 @@
         <v>28</v>
       </c>
       <c r="M128">
-        <v>0.234977874</v>
+        <v>-0.234977874</v>
       </c>
       <c r="N128" t="s">
         <v>25</v>
@@ -10125,7 +10125,7 @@
         <v>28</v>
       </c>
       <c r="M129">
-        <v>0.59511699600000001</v>
+        <v>-0.59511699600000001</v>
       </c>
       <c r="N129" t="s">
         <v>25</v>
@@ -10191,7 +10191,7 @@
         <v>28</v>
       </c>
       <c r="M130">
-        <v>0.34536070499999999</v>
+        <v>-0.34536070499999999</v>
       </c>
       <c r="N130" t="s">
         <v>25</v>
@@ -10257,7 +10257,7 @@
         <v>28</v>
       </c>
       <c r="M131">
-        <v>3.1116305E-2</v>
+        <v>-3.1116305E-2</v>
       </c>
       <c r="N131" t="s">
         <v>25</v>
@@ -10323,7 +10323,7 @@
         <v>28</v>
       </c>
       <c r="M132">
-        <v>-0.612908393</v>
+        <v>0.612908393</v>
       </c>
       <c r="N132" t="s">
         <v>25</v>
@@ -10389,7 +10389,7 @@
         <v>28</v>
       </c>
       <c r="M133">
-        <v>0.41035979700000003</v>
+        <v>-0.41035979700000003</v>
       </c>
       <c r="N133" t="s">
         <v>25</v>
@@ -10455,7 +10455,7 @@
         <v>28</v>
       </c>
       <c r="M134">
-        <v>0.62988575800000002</v>
+        <v>-0.62988575800000002</v>
       </c>
       <c r="N134" t="s">
         <v>25</v>
@@ -10521,7 +10521,7 @@
         <v>28</v>
       </c>
       <c r="M135">
-        <v>0.51947220999999999</v>
+        <v>-0.51947220999999999</v>
       </c>
       <c r="N135" t="s">
         <v>25</v>
@@ -10587,7 +10587,7 @@
         <v>28</v>
       </c>
       <c r="M136">
-        <v>0.64781436599999997</v>
+        <v>-0.64781436599999997</v>
       </c>
       <c r="N136" t="s">
         <v>25</v>
@@ -10653,7 +10653,7 @@
         <v>28</v>
       </c>
       <c r="M137">
-        <v>-0.35542434499999997</v>
+        <v>0.35542434499999997</v>
       </c>
       <c r="N137" t="s">
         <v>25</v>
@@ -10719,7 +10719,7 @@
         <v>28</v>
       </c>
       <c r="M138">
-        <v>-0.12542885200000001</v>
+        <v>0.12542885200000001</v>
       </c>
       <c r="N138" t="s">
         <v>25</v>
@@ -10785,7 +10785,7 @@
         <v>28</v>
       </c>
       <c r="M139">
-        <v>-0.72590231800000005</v>
+        <v>0.72590231800000005</v>
       </c>
       <c r="N139" t="s">
         <v>25</v>
@@ -10851,7 +10851,7 @@
         <v>28</v>
       </c>
       <c r="M140">
-        <v>-2.0473860720000001</v>
+        <v>2.0473860720000001</v>
       </c>
       <c r="N140" t="s">
         <v>25</v>
@@ -10917,7 +10917,7 @@
         <v>28</v>
       </c>
       <c r="M141">
-        <v>0.65505976399999999</v>
+        <v>-0.65505976399999999</v>
       </c>
       <c r="N141" t="s">
         <v>25</v>
@@ -10983,7 +10983,7 @@
         <v>28</v>
       </c>
       <c r="M142">
-        <v>1.2136675299999999</v>
+        <v>-1.2136675299999999</v>
       </c>
       <c r="N142" t="s">
         <v>25</v>
@@ -11049,7 +11049,7 @@
         <v>28</v>
       </c>
       <c r="M143">
-        <v>0.95954067099999996</v>
+        <v>-0.95954067099999996</v>
       </c>
       <c r="N143" t="s">
         <v>25</v>
@@ -11115,7 +11115,7 @@
         <v>28</v>
       </c>
       <c r="M144">
-        <v>-2.4534776360000001</v>
+        <v>2.4534776360000001</v>
       </c>
       <c r="N144" t="s">
         <v>25</v>
@@ -11181,7 +11181,7 @@
         <v>28</v>
       </c>
       <c r="M145">
-        <v>1.055467001</v>
+        <v>-1.055467001</v>
       </c>
       <c r="N145" t="s">
         <v>25</v>
@@ -11247,7 +11247,7 @@
         <v>28</v>
       </c>
       <c r="M146">
-        <v>0.94392273100000001</v>
+        <v>-0.94392273100000001</v>
       </c>
       <c r="N146" t="s">
         <v>25</v>
@@ -11313,7 +11313,7 @@
         <v>28</v>
       </c>
       <c r="M147">
-        <v>0.51638706899999998</v>
+        <v>-0.51638706899999998</v>
       </c>
       <c r="N147" t="s">
         <v>25</v>
@@ -11379,7 +11379,7 @@
         <v>28</v>
       </c>
       <c r="M148">
-        <v>0.38480984699999998</v>
+        <v>-0.38480984699999998</v>
       </c>
       <c r="N148" t="s">
         <v>25</v>
@@ -11445,7 +11445,7 @@
         <v>28</v>
       </c>
       <c r="M149">
-        <v>0.82711900000000005</v>
+        <v>-0.82711900000000005</v>
       </c>
       <c r="N149" t="s">
         <v>25</v>
@@ -11511,7 +11511,7 @@
         <v>28</v>
       </c>
       <c r="M150">
-        <v>1.6178595730000001</v>
+        <v>-1.6178595730000001</v>
       </c>
       <c r="N150" t="s">
         <v>25</v>
@@ -11577,7 +11577,7 @@
         <v>28</v>
       </c>
       <c r="M151">
-        <v>-0.280957913</v>
+        <v>0.280957913</v>
       </c>
       <c r="N151" t="s">
         <v>25</v>
@@ -11643,7 +11643,7 @@
         <v>28</v>
       </c>
       <c r="M152">
-        <v>-2.4494399E-2</v>
+        <v>2.4494399E-2</v>
       </c>
       <c r="N152" t="s">
         <v>25</v>
@@ -11709,7 +11709,7 @@
         <v>28</v>
       </c>
       <c r="M153">
-        <v>1.1510721999999999E-2</v>
+        <v>-1.1510721999999999E-2</v>
       </c>
       <c r="N153" t="s">
         <v>25</v>
@@ -11775,7 +11775,7 @@
         <v>28</v>
       </c>
       <c r="M154">
-        <v>2.8098087000000001E-2</v>
+        <v>-2.8098087000000001E-2</v>
       </c>
       <c r="N154" t="s">
         <v>25</v>
@@ -11841,7 +11841,7 @@
         <v>28</v>
       </c>
       <c r="M155">
-        <v>-0.58328712199999999</v>
+        <v>0.58328712199999999</v>
       </c>
       <c r="N155" t="s">
         <v>25</v>
@@ -11907,7 +11907,7 @@
         <v>28</v>
       </c>
       <c r="M156">
-        <v>-0.20450692600000001</v>
+        <v>0.20450692600000001</v>
       </c>
       <c r="N156" t="s">
         <v>25</v>
@@ -11973,7 +11973,7 @@
         <v>28</v>
       </c>
       <c r="M157">
-        <v>0.488539734</v>
+        <v>-0.488539734</v>
       </c>
       <c r="N157" t="s">
         <v>25</v>
@@ -12039,7 +12039,7 @@
         <v>28</v>
       </c>
       <c r="M158">
-        <v>0.79060392700000004</v>
+        <v>-0.79060392700000004</v>
       </c>
       <c r="N158" t="s">
         <v>25</v>
@@ -12105,7 +12105,7 @@
         <v>28</v>
       </c>
       <c r="M159">
-        <v>0.96164297399999998</v>
+        <v>-0.96164297399999998</v>
       </c>
       <c r="N159" t="s">
         <v>25</v>
@@ -12171,7 +12171,7 @@
         <v>28</v>
       </c>
       <c r="M160">
-        <v>1.769726669</v>
+        <v>-1.769726669</v>
       </c>
       <c r="N160" t="s">
         <v>25</v>
@@ -12237,7 +12237,7 @@
         <v>28</v>
       </c>
       <c r="M161">
-        <v>-0.920882172</v>
+        <v>0.920882172</v>
       </c>
       <c r="N161" t="s">
         <v>25</v>
@@ -12303,7 +12303,7 @@
         <v>28</v>
       </c>
       <c r="M162">
-        <v>-0.67230106199999995</v>
+        <v>0.67230106199999995</v>
       </c>
       <c r="N162" t="s">
         <v>25</v>
@@ -12369,7 +12369,7 @@
         <v>28</v>
       </c>
       <c r="M163">
-        <v>-1.800879924</v>
+        <v>1.800879924</v>
       </c>
       <c r="N163" t="s">
         <v>25</v>
@@ -12435,7 +12435,7 @@
         <v>28</v>
       </c>
       <c r="M164">
-        <v>0.73606665999999998</v>
+        <v>-0.73606665999999998</v>
       </c>
       <c r="N164" t="s">
         <v>25</v>
@@ -12501,7 +12501,7 @@
         <v>28</v>
       </c>
       <c r="M165">
-        <v>0.43799274999999999</v>
+        <v>-0.43799274999999999</v>
       </c>
       <c r="N165" t="s">
         <v>25</v>
@@ -12567,7 +12567,7 @@
         <v>28</v>
       </c>
       <c r="M166">
-        <v>0.50498249100000003</v>
+        <v>-0.50498249100000003</v>
       </c>
       <c r="N166" t="s">
         <v>25</v>
@@ -12633,7 +12633,7 @@
         <v>28</v>
       </c>
       <c r="M167">
-        <v>-0.46726403</v>
+        <v>0.46726403</v>
       </c>
       <c r="N167" t="s">
         <v>25</v>
@@ -12699,7 +12699,7 @@
         <v>28</v>
       </c>
       <c r="M168">
-        <v>0.91871855800000002</v>
+        <v>-0.91871855800000002</v>
       </c>
       <c r="N168" t="s">
         <v>25</v>
@@ -12765,7 +12765,7 @@
         <v>28</v>
       </c>
       <c r="M169">
-        <v>-8.4895709999999999E-2</v>
+        <v>8.4895709999999999E-2</v>
       </c>
       <c r="N169" t="s">
         <v>25</v>
@@ -12831,7 +12831,7 @@
         <v>28</v>
       </c>
       <c r="M170">
-        <v>0.61966960199999999</v>
+        <v>-0.61966960199999999</v>
       </c>
       <c r="N170" t="s">
         <v>25</v>
@@ -12897,7 +12897,7 @@
         <v>28</v>
       </c>
       <c r="M171">
-        <v>1.620157922</v>
+        <v>-1.620157922</v>
       </c>
       <c r="N171" t="s">
         <v>25</v>
@@ -12963,7 +12963,7 @@
         <v>28</v>
       </c>
       <c r="M172">
-        <v>-2.4303435019999999</v>
+        <v>2.4303435019999999</v>
       </c>
       <c r="N172" t="s">
         <v>25</v>
@@ -13029,7 +13029,7 @@
         <v>28</v>
       </c>
       <c r="M173">
-        <v>-0.41009677999999999</v>
+        <v>0.41009677999999999</v>
       </c>
       <c r="N173" t="s">
         <v>25</v>
@@ -13095,7 +13095,7 @@
         <v>28</v>
       </c>
       <c r="M174">
-        <v>-0.141873993</v>
+        <v>0.141873993</v>
       </c>
       <c r="N174" t="s">
         <v>25</v>
@@ -13161,7 +13161,7 @@
         <v>28</v>
       </c>
       <c r="M175">
-        <v>0.50873493400000003</v>
+        <v>-0.50873493400000003</v>
       </c>
       <c r="N175" t="s">
         <v>25</v>
@@ -13227,7 +13227,7 @@
         <v>28</v>
       </c>
       <c r="M176">
-        <v>0.91052793600000004</v>
+        <v>-0.91052793600000004</v>
       </c>
       <c r="N176" t="s">
         <v>25</v>
@@ -13293,7 +13293,7 @@
         <v>28</v>
       </c>
       <c r="M177">
-        <v>0.307965555</v>
+        <v>-0.307965555</v>
       </c>
       <c r="N177" t="s">
         <v>25</v>
@@ -13359,7 +13359,7 @@
         <v>28</v>
       </c>
       <c r="M178">
-        <v>-0.27195224099999998</v>
+        <v>0.27195224099999998</v>
       </c>
       <c r="N178" t="s">
         <v>25</v>
@@ -13425,7 +13425,7 @@
         <v>28</v>
       </c>
       <c r="M179">
-        <v>0.22031584800000001</v>
+        <v>-0.22031584800000001</v>
       </c>
       <c r="N179" t="s">
         <v>25</v>
@@ -13491,7 +13491,7 @@
         <v>28</v>
       </c>
       <c r="M180">
-        <v>0.80560845299999995</v>
+        <v>-0.80560845299999995</v>
       </c>
       <c r="N180" t="s">
         <v>25</v>
@@ -13557,7 +13557,7 @@
         <v>28</v>
       </c>
       <c r="M181">
-        <v>-1.261370203</v>
+        <v>1.261370203</v>
       </c>
       <c r="N181" t="s">
         <v>25</v>
@@ -13623,7 +13623,7 @@
         <v>28</v>
       </c>
       <c r="M182">
-        <v>-0.10682037799999999</v>
+        <v>0.10682037799999999</v>
       </c>
       <c r="N182" t="s">
         <v>25</v>
@@ -13689,7 +13689,7 @@
         <v>28</v>
       </c>
       <c r="M183">
-        <v>0.18073494200000001</v>
+        <v>-0.18073494200000001</v>
       </c>
       <c r="N183" t="s">
         <v>25</v>
@@ -13755,7 +13755,7 @@
         <v>28</v>
       </c>
       <c r="M184">
-        <v>1.2624031790000001</v>
+        <v>-1.2624031790000001</v>
       </c>
       <c r="N184" t="s">
         <v>25</v>
@@ -13821,7 +13821,7 @@
         <v>28</v>
       </c>
       <c r="M185">
-        <v>0.63325131899999998</v>
+        <v>-0.63325131899999998</v>
       </c>
       <c r="N185" t="s">
         <v>25</v>
@@ -13887,7 +13887,7 @@
         <v>28</v>
       </c>
       <c r="M186">
-        <v>-0.76787245299999995</v>
+        <v>0.76787245299999995</v>
       </c>
       <c r="N186" t="s">
         <v>25</v>
@@ -13953,7 +13953,7 @@
         <v>28</v>
       </c>
       <c r="M187">
-        <v>-1.536525766</v>
+        <v>1.536525766</v>
       </c>
       <c r="N187" t="s">
         <v>25</v>
@@ -14019,7 +14019,7 @@
         <v>28</v>
       </c>
       <c r="M188">
-        <v>-0.34926300300000002</v>
+        <v>0.34926300300000002</v>
       </c>
       <c r="N188" t="s">
         <v>25</v>
@@ -14085,7 +14085,7 @@
         <v>28</v>
       </c>
       <c r="M189">
-        <v>-1.0603655540000001</v>
+        <v>1.0603655540000001</v>
       </c>
       <c r="N189" t="s">
         <v>25</v>
@@ -14151,7 +14151,7 @@
         <v>28</v>
       </c>
       <c r="M190">
-        <v>-0.59537201299999998</v>
+        <v>0.59537201299999998</v>
       </c>
       <c r="N190" t="s">
         <v>25</v>
@@ -14217,7 +14217,7 @@
         <v>28</v>
       </c>
       <c r="M191">
-        <v>0.80341889499999997</v>
+        <v>-0.80341889499999997</v>
       </c>
       <c r="N191" t="s">
         <v>25</v>
@@ -14283,7 +14283,7 @@
         <v>28</v>
       </c>
       <c r="M192">
-        <v>0.725711879</v>
+        <v>-0.725711879</v>
       </c>
       <c r="N192" t="s">
         <v>25</v>
@@ -14349,7 +14349,7 @@
         <v>28</v>
       </c>
       <c r="M193">
-        <v>-0.32411310599999998</v>
+        <v>0.32411310599999998</v>
       </c>
       <c r="N193" t="s">
         <v>25</v>
@@ -14415,7 +14415,7 @@
         <v>28</v>
       </c>
       <c r="M194">
-        <v>-0.72765014699999997</v>
+        <v>0.72765014699999997</v>
       </c>
       <c r="N194" t="s">
         <v>25</v>
@@ -14481,7 +14481,7 @@
         <v>28</v>
       </c>
       <c r="M195">
-        <v>-0.99064947000000003</v>
+        <v>0.99064947000000003</v>
       </c>
       <c r="N195" t="s">
         <v>25</v>
@@ -14547,7 +14547,7 @@
         <v>28</v>
       </c>
       <c r="M196">
-        <v>0.61885697799999995</v>
+        <v>-0.61885697799999995</v>
       </c>
       <c r="N196" t="s">
         <v>25</v>
@@ -14613,7 +14613,7 @@
         <v>28</v>
       </c>
       <c r="M197">
-        <v>-0.16809634500000001</v>
+        <v>0.16809634500000001</v>
       </c>
       <c r="N197" t="s">
         <v>25</v>
@@ -14679,7 +14679,7 @@
         <v>28</v>
       </c>
       <c r="M198">
-        <v>-0.78469254200000005</v>
+        <v>0.78469254200000005</v>
       </c>
       <c r="N198" t="s">
         <v>25</v>
@@ -14745,7 +14745,7 @@
         <v>28</v>
       </c>
       <c r="M199">
-        <v>0.53032917700000004</v>
+        <v>-0.53032917700000004</v>
       </c>
       <c r="N199" t="s">
         <v>25</v>
@@ -14811,7 +14811,7 @@
         <v>28</v>
       </c>
       <c r="M200">
-        <v>-0.89195134799999998</v>
+        <v>0.89195134799999998</v>
       </c>
       <c r="N200" t="s">
         <v>25</v>
@@ -14877,7 +14877,7 @@
         <v>28</v>
       </c>
       <c r="M201">
-        <v>0.80875319199999995</v>
+        <v>-0.80875319199999995</v>
       </c>
       <c r="N201" t="s">
         <v>25</v>
@@ -14943,7 +14943,7 @@
         <v>28</v>
       </c>
       <c r="M202">
-        <v>-0.57184811199999996</v>
+        <v>0.57184811199999996</v>
       </c>
       <c r="N202" t="s">
         <v>25</v>
@@ -15009,7 +15009,7 @@
         <v>28</v>
       </c>
       <c r="M203">
-        <v>0.35347940100000003</v>
+        <v>-0.35347940100000003</v>
       </c>
       <c r="N203" t="s">
         <v>25</v>
@@ -15075,7 +15075,7 @@
         <v>28</v>
       </c>
       <c r="M204">
-        <v>-0.170384111</v>
+        <v>0.170384111</v>
       </c>
       <c r="N204" t="s">
         <v>25</v>

</xml_diff>